<commit_message>
updated bowtie script template
</commit_message>
<xml_diff>
--- a/sponge scripts.xlsx
+++ b/sponge scripts.xlsx
@@ -5,23 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Cvarians/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.studivan/Downloads/Cvarians/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23AB953-60A6-8049-979B-28BF7C998CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DB2DFC-21AE-124D-BBDF-B892DADC8D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20240" activeTab="8" xr2:uid="{000E1DAA-3B9E-6A49-A3E6-11DA32F9C3E6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20240" activeTab="5" xr2:uid="{000E1DAA-3B9E-6A49-A3E6-11DA32F9C3E6}"/>
   </bookViews>
   <sheets>
     <sheet name="repair" sheetId="1" r:id="rId1"/>
     <sheet name="dedup" sheetId="2" r:id="rId2"/>
     <sheet name="concat" sheetId="3" r:id="rId3"/>
     <sheet name="pione bowtie" sheetId="4" r:id="rId4"/>
-    <sheet name="bowtie" sheetId="5" r:id="rId5"/>
-    <sheet name="bowtie2" sheetId="7" r:id="rId6"/>
-    <sheet name="bowtie3" sheetId="9" r:id="rId7"/>
-    <sheet name="bowtie4" sheetId="10" r:id="rId8"/>
-    <sheet name="bowtie5" sheetId="11" r:id="rId9"/>
+    <sheet name="cliona bowtie" sheetId="5" r:id="rId5"/>
+    <sheet name="cliona bowtie2" sheetId="7" r:id="rId6"/>
+    <sheet name="cliona bowtie3" sheetId="10" r:id="rId7"/>
+    <sheet name="cliona bowtie4" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="1019">
   <si>
     <t>Cliona_10_S8_L001_R1_001.trim</t>
   </si>
@@ -2417,213 +2416,6 @@
     <t>Cliona_Redo9.fastq.host.un</t>
   </si>
   <si>
-    <t>Cliona_10.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_17.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_1.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_21.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_22.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_23.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_4.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_5.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_6.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_8.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_9.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo10.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo11.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo12.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo13.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo1.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo2.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo3.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo4.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo5.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo7.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo8.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_Redo9.fastq.host.clean.sam</t>
-  </si>
-  <si>
-    <t>Cliona_10.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_17.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_1.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_21.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_22.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_23.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_4.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_5.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_6.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_8.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_9.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo10.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo11.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo12.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo13.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo1.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo2.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo3.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo4.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo5.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo7.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo8.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo9.fastq.host.1.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo9.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_10.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_17.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_1.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_21.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_22.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_23.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_4.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_5.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_6.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_8.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_9.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo10.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo11.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo12.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo13.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo1.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo2.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo3.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo4.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo5.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo7.fastq.host.2.clean</t>
-  </si>
-  <si>
-    <t>Cliona_Redo8.fastq.host.2.clean</t>
-  </si>
-  <si>
     <t>Cliona_10.fastq.sym.sam</t>
   </si>
   <si>
@@ -3174,6 +2966,138 @@
   </si>
   <si>
     <t>Cliona_Redo9.fastq.sym.2.clean</t>
+  </si>
+  <si>
+    <t>Pione_1.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_10.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_11.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_12.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_13.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_14.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_15.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_17.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_18.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_19.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_2.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_20.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_21.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_23.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_24.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_3.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_4.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_5.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_6.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_7.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_8.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_9.fastq.clean</t>
+  </si>
+  <si>
+    <t>Pione_1.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_10.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_11.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_12.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_13.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_14.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_15.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_17.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_18.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_19.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_2.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_20.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_21.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_23.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_24.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_3.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_4.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_5.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_6.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_7.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_8.fastq.un</t>
+  </si>
+  <si>
+    <t>Pione_9.fastq.un</t>
   </si>
 </sst>
 </file>
@@ -6495,324 +6419,460 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21FFFB0E-EC30-0D44-BA87-EA0D3EAEA50B}">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A1:XFD1048576"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>539</v>
       </c>
       <c r="C1" t="s">
         <v>495</v>
       </c>
-      <c r="F1" t="str">
-        <f>("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 "&amp;C1&amp;" -2 "&amp;C23&amp;" -S "&amp;A1&amp;" --no-hd --no-sq --no-unal")</f>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_1.fastq -2 R2_Pione_1.fastq -S Pione_1.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>975</v>
+      </c>
+      <c r="H1" t="s">
+        <v>997</v>
+      </c>
+      <c r="J1" t="str">
+        <f>("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 "&amp;C1&amp;" -2 "&amp;C23&amp;" -S "&amp;A1&amp;" --no-hd --no-sq --no-unal --al-conc ./"&amp;F1&amp;" --un-conc junk/"&amp;H1)</f>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_1.fastq -2 R2_Pione_1.fastq -S Pione_1.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_1.fastq.clean --un-conc junk/Pione_1.fastq.un</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>540</v>
       </c>
       <c r="C2" t="s">
         <v>496</v>
       </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F22" si="0">("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 "&amp;C2&amp;" -2 "&amp;C24&amp;" -S "&amp;A2&amp;" --no-hd --no-sq --no-unal")</f>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_10.fastq -2 R2_Pione_10.fastq -S Pione_10.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>976</v>
+      </c>
+      <c r="H2" t="s">
+        <v>998</v>
+      </c>
+      <c r="J2" t="str">
+        <f t="shared" ref="J2:J22" si="0">("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 "&amp;C2&amp;" -2 "&amp;C24&amp;" -S "&amp;A2&amp;" --no-hd --no-sq --no-unal --al-conc ./"&amp;F2&amp;" --un-conc junk/"&amp;H2)</f>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_10.fastq -2 R2_Pione_10.fastq -S Pione_10.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_10.fastq.clean --un-conc junk/Pione_10.fastq.un</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>541</v>
       </c>
       <c r="C3" t="s">
         <v>497</v>
       </c>
-      <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_11.fastq -2 R2_Pione_11.fastq -S Pione_11.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>977</v>
+      </c>
+      <c r="H3" t="s">
+        <v>999</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_11.fastq -2 R2_Pione_11.fastq -S Pione_11.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_11.fastq.clean --un-conc junk/Pione_11.fastq.un</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>542</v>
       </c>
       <c r="C4" t="s">
         <v>498</v>
       </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_12.fastq -2 R2_Pione_12.fastq -S Pione_12.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>978</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1000</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_12.fastq -2 R2_Pione_12.fastq -S Pione_12.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_12.fastq.clean --un-conc junk/Pione_12.fastq.un</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>543</v>
       </c>
       <c r="C5" t="s">
         <v>499</v>
       </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_13.fastq -2 R2_Pione_13.fastq -S Pione_13.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>979</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_13.fastq -2 R2_Pione_13.fastq -S Pione_13.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_13.fastq.clean --un-conc junk/Pione_13.fastq.un</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>544</v>
       </c>
       <c r="C6" t="s">
         <v>500</v>
       </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_14.fastq -2 R2_Pione_14.fastq -S Pione_14.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>980</v>
+      </c>
+      <c r="H6" t="s">
+        <v>1002</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_14.fastq -2 R2_Pione_14.fastq -S Pione_14.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_14.fastq.clean --un-conc junk/Pione_14.fastq.un</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>545</v>
       </c>
       <c r="C7" t="s">
         <v>501</v>
       </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_15.fastq -2 R2_Pione_15.fastq -S Pione_15.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>981</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_15.fastq -2 R2_Pione_15.fastq -S Pione_15.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_15.fastq.clean --un-conc junk/Pione_15.fastq.un</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>546</v>
       </c>
       <c r="C8" t="s">
         <v>502</v>
       </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_17.fastq -2 R2_Pione_17.fastq -S Pione_17.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>982</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1004</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_17.fastq -2 R2_Pione_17.fastq -S Pione_17.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_17.fastq.clean --un-conc junk/Pione_17.fastq.un</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>547</v>
       </c>
       <c r="C9" t="s">
         <v>503</v>
       </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_18.fastq -2 R2_Pione_18.fastq -S Pione_18.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>983</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1005</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_18.fastq -2 R2_Pione_18.fastq -S Pione_18.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_18.fastq.clean --un-conc junk/Pione_18.fastq.un</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>548</v>
       </c>
       <c r="C10" t="s">
         <v>504</v>
       </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_19.fastq -2 R2_Pione_19.fastq -S Pione_19.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>984</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1006</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_19.fastq -2 R2_Pione_19.fastq -S Pione_19.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_19.fastq.clean --un-conc junk/Pione_19.fastq.un</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>549</v>
       </c>
       <c r="C11" t="s">
         <v>505</v>
       </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_2.fastq -2 R2_Pione_2.fastq -S Pione_2.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>985</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1007</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_2.fastq -2 R2_Pione_2.fastq -S Pione_2.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_2.fastq.clean --un-conc junk/Pione_2.fastq.un</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>550</v>
       </c>
       <c r="C12" t="s">
         <v>506</v>
       </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_20.fastq -2 R2_Pione_20.fastq -S Pione_20.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>986</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1008</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_20.fastq -2 R2_Pione_20.fastq -S Pione_20.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_20.fastq.clean --un-conc junk/Pione_20.fastq.un</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>551</v>
       </c>
       <c r="C13" t="s">
         <v>507</v>
       </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_21.fastq -2 R2_Pione_21.fastq -S Pione_21.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>987</v>
+      </c>
+      <c r="H13" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_21.fastq -2 R2_Pione_21.fastq -S Pione_21.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_21.fastq.clean --un-conc junk/Pione_21.fastq.un</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>552</v>
       </c>
       <c r="C14" t="s">
         <v>508</v>
       </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_23.fastq -2 R2_Pione_23.fastq -S Pione_23.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>988</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1010</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_23.fastq -2 R2_Pione_23.fastq -S Pione_23.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_23.fastq.clean --un-conc junk/Pione_23.fastq.un</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>553</v>
       </c>
       <c r="C15" t="s">
         <v>509</v>
       </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_24.fastq -2 R2_Pione_24.fastq -S Pione_24.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>989</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1011</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_24.fastq -2 R2_Pione_24.fastq -S Pione_24.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_24.fastq.clean --un-conc junk/Pione_24.fastq.un</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>554</v>
       </c>
       <c r="C16" t="s">
         <v>510</v>
       </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_3.fastq -2 R2_Pione_3.fastq -S Pione_3.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>990</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1012</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_3.fastq -2 R2_Pione_3.fastq -S Pione_3.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_3.fastq.clean --un-conc junk/Pione_3.fastq.un</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>555</v>
       </c>
       <c r="C17" t="s">
         <v>511</v>
       </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_4.fastq -2 R2_Pione_4.fastq -S Pione_4.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>991</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1013</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_4.fastq -2 R2_Pione_4.fastq -S Pione_4.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_4.fastq.clean --un-conc junk/Pione_4.fastq.un</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>556</v>
       </c>
       <c r="C18" t="s">
         <v>512</v>
       </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_5.fastq -2 R2_Pione_5.fastq -S Pione_5.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>992</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1014</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_5.fastq -2 R2_Pione_5.fastq -S Pione_5.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_5.fastq.clean --un-conc junk/Pione_5.fastq.un</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>557</v>
       </c>
       <c r="C19" t="s">
         <v>513</v>
       </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_6.fastq -2 R2_Pione_6.fastq -S Pione_6.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>993</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1015</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_6.fastq -2 R2_Pione_6.fastq -S Pione_6.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_6.fastq.clean --un-conc junk/Pione_6.fastq.un</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>558</v>
       </c>
       <c r="C20" t="s">
         <v>514</v>
       </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_7.fastq -2 R2_Pione_7.fastq -S Pione_7.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>994</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1016</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_7.fastq -2 R2_Pione_7.fastq -S Pione_7.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_7.fastq.clean --un-conc junk/Pione_7.fastq.un</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>559</v>
       </c>
       <c r="C21" t="s">
         <v>515</v>
       </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_8.fastq -2 R2_Pione_8.fastq -S Pione_8.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>995</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_8.fastq -2 R2_Pione_8.fastq -S Pione_8.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_8.fastq.clean --un-conc junk/Pione_8.fastq.un</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>560</v>
       </c>
       <c r="C22" t="s">
         <v>516</v>
       </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_9.fastq -2 R2_Pione_9.fastq -S Pione_9.fastq.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>996</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1018</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" si="0"/>
+        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Plampa -1 R1_Pione_9.fastq -2 R2_Pione_9.fastq -S Pione_9.fastq.sam --no-hd --no-sq --no-unal --al-conc ./Pione_9.fastq.clean --un-conc junk/Pione_9.fastq.un</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>522</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>526</v>
       </c>
@@ -7430,8 +7490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65592D39-BD28-0343-857C-11FA77A84A03}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G25" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7977,420 +8037,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A32A60-9E67-5A45-927E-48F8C8984D59}">
-  <dimension ref="A1:F46"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J42" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>791</v>
-      </c>
-      <c r="C1" t="s">
-        <v>814</v>
-      </c>
-      <c r="F1" t="str">
-        <f>("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 "&amp;C1&amp;" -2 "&amp;C24&amp;" -S "&amp;A1&amp;" --no-hd --no-sq --no-unal")</f>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_10.fastq.host.1.clean -2 Cliona_10.fastq.host.2.clean -S Cliona_10.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>792</v>
-      </c>
-      <c r="C2" t="s">
-        <v>815</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F23" si="0">("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 "&amp;C2&amp;" -2 "&amp;C25&amp;" -S "&amp;A2&amp;" --no-hd --no-sq --no-unal")</f>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_17.fastq.host.1.clean -2 Cliona_17.fastq.host.2.clean -S Cliona_17.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>793</v>
-      </c>
-      <c r="C3" t="s">
-        <v>816</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_1.fastq.host.1.clean -2 Cliona_1.fastq.host.2.clean -S Cliona_1.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>794</v>
-      </c>
-      <c r="C4" t="s">
-        <v>817</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_21.fastq.host.1.clean -2 Cliona_21.fastq.host.2.clean -S Cliona_21.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>795</v>
-      </c>
-      <c r="C5" t="s">
-        <v>818</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_22.fastq.host.1.clean -2 Cliona_22.fastq.host.2.clean -S Cliona_22.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>796</v>
-      </c>
-      <c r="C6" t="s">
-        <v>819</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_23.fastq.host.1.clean -2 Cliona_23.fastq.host.2.clean -S Cliona_23.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>797</v>
-      </c>
-      <c r="C7" t="s">
-        <v>820</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_4.fastq.host.1.clean -2 Cliona_4.fastq.host.2.clean -S Cliona_4.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>798</v>
-      </c>
-      <c r="C8" t="s">
-        <v>821</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_5.fastq.host.1.clean -2 Cliona_5.fastq.host.2.clean -S Cliona_5.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>799</v>
-      </c>
-      <c r="C9" t="s">
-        <v>822</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_6.fastq.host.1.clean -2 Cliona_6.fastq.host.2.clean -S Cliona_6.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>800</v>
-      </c>
-      <c r="C10" t="s">
-        <v>823</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_8.fastq.host.1.clean -2 Cliona_8.fastq.host.2.clean -S Cliona_8.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>801</v>
-      </c>
-      <c r="C11" t="s">
-        <v>824</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_9.fastq.host.1.clean -2 Cliona_9.fastq.host.2.clean -S Cliona_9.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>802</v>
-      </c>
-      <c r="C12" t="s">
-        <v>825</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo10.fastq.host.1.clean -2 Cliona_Redo10.fastq.host.2.clean -S Cliona_Redo10.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>803</v>
-      </c>
-      <c r="C13" t="s">
-        <v>826</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo11.fastq.host.1.clean -2 Cliona_Redo11.fastq.host.2.clean -S Cliona_Redo11.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>804</v>
-      </c>
-      <c r="C14" t="s">
-        <v>827</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo12.fastq.host.1.clean -2 Cliona_Redo12.fastq.host.2.clean -S Cliona_Redo12.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>805</v>
-      </c>
-      <c r="C15" t="s">
-        <v>828</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo13.fastq.host.1.clean -2 Cliona_Redo13.fastq.host.2.clean -S Cliona_Redo13.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>806</v>
-      </c>
-      <c r="C16" t="s">
-        <v>829</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo1.fastq.host.1.clean -2 Cliona_Redo1.fastq.host.2.clean -S Cliona_Redo1.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>807</v>
-      </c>
-      <c r="C17" t="s">
-        <v>830</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo2.fastq.host.1.clean -2 Cliona_Redo2.fastq.host.2.clean -S Cliona_Redo2.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>808</v>
-      </c>
-      <c r="C18" t="s">
-        <v>831</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo3.fastq.host.1.clean -2 Cliona_Redo3.fastq.host.2.clean -S Cliona_Redo3.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>809</v>
-      </c>
-      <c r="C19" t="s">
-        <v>832</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo4.fastq.host.1.clean -2 Cliona_Redo4.fastq.host.2.clean -S Cliona_Redo4.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>810</v>
-      </c>
-      <c r="C20" t="s">
-        <v>833</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo5.fastq.host.1.clean -2 Cliona_Redo5.fastq.host.2.clean -S Cliona_Redo5.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>811</v>
-      </c>
-      <c r="C21" t="s">
-        <v>834</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo7.fastq.host.1.clean -2 Cliona_Redo7.fastq.host.2.clean -S Cliona_Redo7.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>812</v>
-      </c>
-      <c r="C22" t="s">
-        <v>835</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo8.fastq.host.1.clean -2 Cliona_Redo8.fastq.host.2.clean -S Cliona_Redo8.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>813</v>
-      </c>
-      <c r="C23" t="s">
-        <v>836</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="0"/>
-        <v>bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 Cliona_Redo9.fastq.host.1.clean -2 Cliona_Redo9.fastq.host.2.clean -S Cliona_Redo9.fastq.host.clean.sam --no-hd --no-sq --no-unal</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C46" t="s">
-        <v>837</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B582F1-67F7-F04C-9CEC-744B05445545}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
@@ -8404,16 +8054,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>791</v>
+      </c>
+      <c r="C1" t="s">
+        <v>814</v>
+      </c>
+      <c r="E1" t="s">
         <v>860</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>883</v>
-      </c>
-      <c r="E1" t="s">
-        <v>929</v>
-      </c>
-      <c r="G1" t="s">
-        <v>952</v>
       </c>
       <c r="I1" t="str">
         <f>("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 "&amp;C1&amp;" -2 "&amp;C24&amp;" -S "&amp;A1&amp;" --no-hd --no-sq --no-unal --al-conc ./"&amp;E1&amp;" --un-conc junk/"&amp;G1)</f>
@@ -8422,16 +8072,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>792</v>
+      </c>
+      <c r="C2" t="s">
+        <v>815</v>
+      </c>
+      <c r="E2" t="s">
         <v>861</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>884</v>
-      </c>
-      <c r="E2" t="s">
-        <v>930</v>
-      </c>
-      <c r="G2" t="s">
-        <v>953</v>
       </c>
       <c r="I2" t="str">
         <f t="shared" ref="I2:I23" si="0">("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Cvarians -1 "&amp;C2&amp;" -2 "&amp;C25&amp;" -S "&amp;A2&amp;" --no-hd --no-sq --no-unal --al-conc ./"&amp;E2&amp;" --un-conc junk/"&amp;G2)</f>
@@ -8440,16 +8090,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>793</v>
+      </c>
+      <c r="C3" t="s">
+        <v>816</v>
+      </c>
+      <c r="E3" t="s">
         <v>862</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>885</v>
-      </c>
-      <c r="E3" t="s">
-        <v>931</v>
-      </c>
-      <c r="G3" t="s">
-        <v>954</v>
       </c>
       <c r="I3" t="str">
         <f t="shared" si="0"/>
@@ -8458,16 +8108,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>794</v>
+      </c>
+      <c r="C4" t="s">
+        <v>817</v>
+      </c>
+      <c r="E4" t="s">
         <v>863</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>886</v>
-      </c>
-      <c r="E4" t="s">
-        <v>932</v>
-      </c>
-      <c r="G4" t="s">
-        <v>955</v>
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
@@ -8476,16 +8126,16 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>795</v>
+      </c>
+      <c r="C5" t="s">
+        <v>818</v>
+      </c>
+      <c r="E5" t="s">
         <v>864</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>887</v>
-      </c>
-      <c r="E5" t="s">
-        <v>933</v>
-      </c>
-      <c r="G5" t="s">
-        <v>956</v>
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
@@ -8494,16 +8144,16 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>796</v>
+      </c>
+      <c r="C6" t="s">
+        <v>819</v>
+      </c>
+      <c r="E6" t="s">
         <v>865</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>888</v>
-      </c>
-      <c r="E6" t="s">
-        <v>934</v>
-      </c>
-      <c r="G6" t="s">
-        <v>957</v>
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
@@ -8512,16 +8162,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>797</v>
+      </c>
+      <c r="C7" t="s">
+        <v>820</v>
+      </c>
+      <c r="E7" t="s">
         <v>866</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
         <v>889</v>
-      </c>
-      <c r="E7" t="s">
-        <v>935</v>
-      </c>
-      <c r="G7" t="s">
-        <v>958</v>
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
@@ -8530,16 +8180,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>798</v>
+      </c>
+      <c r="C8" t="s">
+        <v>821</v>
+      </c>
+      <c r="E8" t="s">
         <v>867</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
         <v>890</v>
-      </c>
-      <c r="E8" t="s">
-        <v>936</v>
-      </c>
-      <c r="G8" t="s">
-        <v>959</v>
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
@@ -8548,16 +8198,16 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>799</v>
+      </c>
+      <c r="C9" t="s">
+        <v>822</v>
+      </c>
+      <c r="E9" t="s">
         <v>868</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" t="s">
         <v>891</v>
-      </c>
-      <c r="E9" t="s">
-        <v>937</v>
-      </c>
-      <c r="G9" t="s">
-        <v>960</v>
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
@@ -8566,16 +8216,16 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>800</v>
+      </c>
+      <c r="C10" t="s">
+        <v>823</v>
+      </c>
+      <c r="E10" t="s">
         <v>869</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>892</v>
-      </c>
-      <c r="E10" t="s">
-        <v>938</v>
-      </c>
-      <c r="G10" t="s">
-        <v>961</v>
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
@@ -8584,16 +8234,16 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>801</v>
+      </c>
+      <c r="C11" t="s">
+        <v>824</v>
+      </c>
+      <c r="E11" t="s">
         <v>870</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
         <v>893</v>
-      </c>
-      <c r="E11" t="s">
-        <v>939</v>
-      </c>
-      <c r="G11" t="s">
-        <v>962</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
@@ -8602,16 +8252,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>802</v>
+      </c>
+      <c r="C12" t="s">
+        <v>825</v>
+      </c>
+      <c r="E12" t="s">
         <v>871</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>894</v>
-      </c>
-      <c r="E12" t="s">
-        <v>940</v>
-      </c>
-      <c r="G12" t="s">
-        <v>963</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
@@ -8620,16 +8270,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>803</v>
+      </c>
+      <c r="C13" t="s">
+        <v>826</v>
+      </c>
+      <c r="E13" t="s">
         <v>872</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>895</v>
-      </c>
-      <c r="E13" t="s">
-        <v>941</v>
-      </c>
-      <c r="G13" t="s">
-        <v>964</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
@@ -8638,16 +8288,16 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>804</v>
+      </c>
+      <c r="C14" t="s">
+        <v>827</v>
+      </c>
+      <c r="E14" t="s">
         <v>873</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
         <v>896</v>
-      </c>
-      <c r="E14" t="s">
-        <v>942</v>
-      </c>
-      <c r="G14" t="s">
-        <v>965</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
@@ -8656,16 +8306,16 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>805</v>
+      </c>
+      <c r="C15" t="s">
+        <v>828</v>
+      </c>
+      <c r="E15" t="s">
         <v>874</v>
       </c>
-      <c r="C15" t="s">
+      <c r="G15" t="s">
         <v>897</v>
-      </c>
-      <c r="E15" t="s">
-        <v>943</v>
-      </c>
-      <c r="G15" t="s">
-        <v>966</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
@@ -8674,16 +8324,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>806</v>
+      </c>
+      <c r="C16" t="s">
+        <v>829</v>
+      </c>
+      <c r="E16" t="s">
         <v>875</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16" t="s">
         <v>898</v>
-      </c>
-      <c r="E16" t="s">
-        <v>944</v>
-      </c>
-      <c r="G16" t="s">
-        <v>967</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
@@ -8692,16 +8342,16 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>807</v>
+      </c>
+      <c r="C17" t="s">
+        <v>830</v>
+      </c>
+      <c r="E17" t="s">
         <v>876</v>
       </c>
-      <c r="C17" t="s">
+      <c r="G17" t="s">
         <v>899</v>
-      </c>
-      <c r="E17" t="s">
-        <v>945</v>
-      </c>
-      <c r="G17" t="s">
-        <v>968</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
@@ -8710,16 +8360,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>808</v>
+      </c>
+      <c r="C18" t="s">
+        <v>831</v>
+      </c>
+      <c r="E18" t="s">
         <v>877</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G18" t="s">
         <v>900</v>
-      </c>
-      <c r="E18" t="s">
-        <v>946</v>
-      </c>
-      <c r="G18" t="s">
-        <v>969</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
@@ -8728,16 +8378,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>809</v>
+      </c>
+      <c r="C19" t="s">
+        <v>832</v>
+      </c>
+      <c r="E19" t="s">
         <v>878</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G19" t="s">
         <v>901</v>
-      </c>
-      <c r="E19" t="s">
-        <v>947</v>
-      </c>
-      <c r="G19" t="s">
-        <v>970</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
@@ -8746,16 +8396,16 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>810</v>
+      </c>
+      <c r="C20" t="s">
+        <v>833</v>
+      </c>
+      <c r="E20" t="s">
         <v>879</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" t="s">
         <v>902</v>
-      </c>
-      <c r="E20" t="s">
-        <v>948</v>
-      </c>
-      <c r="G20" t="s">
-        <v>971</v>
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
@@ -8764,16 +8414,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>811</v>
+      </c>
+      <c r="C21" t="s">
+        <v>834</v>
+      </c>
+      <c r="E21" t="s">
         <v>880</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G21" t="s">
         <v>903</v>
-      </c>
-      <c r="E21" t="s">
-        <v>949</v>
-      </c>
-      <c r="G21" t="s">
-        <v>972</v>
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
@@ -8782,16 +8432,16 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>812</v>
+      </c>
+      <c r="C22" t="s">
+        <v>835</v>
+      </c>
+      <c r="E22" t="s">
         <v>881</v>
       </c>
-      <c r="C22" t="s">
+      <c r="G22" t="s">
         <v>904</v>
-      </c>
-      <c r="E22" t="s">
-        <v>950</v>
-      </c>
-      <c r="G22" t="s">
-        <v>973</v>
       </c>
       <c r="I22" t="str">
         <f t="shared" si="0"/>
@@ -8800,16 +8450,16 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>813</v>
+      </c>
+      <c r="C23" t="s">
+        <v>836</v>
+      </c>
+      <c r="E23" t="s">
         <v>882</v>
       </c>
-      <c r="C23" t="s">
+      <c r="G23" t="s">
         <v>905</v>
-      </c>
-      <c r="E23" t="s">
-        <v>951</v>
-      </c>
-      <c r="G23" t="s">
-        <v>974</v>
       </c>
       <c r="I23" t="str">
         <f t="shared" si="0"/>
@@ -8818,117 +8468,117 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>906</v>
+        <v>837</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>907</v>
+        <v>838</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>908</v>
+        <v>839</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>909</v>
+        <v>840</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>910</v>
+        <v>841</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>911</v>
+        <v>842</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>912</v>
+        <v>843</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>913</v>
+        <v>844</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>914</v>
+        <v>845</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>915</v>
+        <v>846</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>916</v>
+        <v>847</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>917</v>
+        <v>848</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>918</v>
+        <v>849</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>919</v>
+        <v>850</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>920</v>
+        <v>851</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>921</v>
+        <v>852</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>922</v>
+        <v>853</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>923</v>
+        <v>854</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>924</v>
+        <v>855</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>925</v>
+        <v>856</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>926</v>
+        <v>857</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>927</v>
+        <v>858</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>928</v>
+        <v>859</v>
       </c>
     </row>
   </sheetData>
@@ -8936,12 +8586,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A558AE64-955A-934A-BD86-254304716E54}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8952,10 +8602,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>975</v>
+        <v>906</v>
       </c>
       <c r="C1" t="s">
-        <v>976</v>
+        <v>907</v>
       </c>
       <c r="F1" t="str">
         <f>("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Gerakladium -1 "&amp;C1&amp;" -2 "&amp;C24&amp;" -S "&amp;A1&amp;" --no-hd --no-sq --no-unal")</f>
@@ -8964,10 +8614,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>977</v>
+        <v>908</v>
       </c>
       <c r="C2" t="s">
-        <v>978</v>
+        <v>909</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F23" si="0">("bowtie2 --local -x /mnt/beegfs/home/mstudiva/db/Gerakladium -1 "&amp;C2&amp;" -2 "&amp;C25&amp;" -S "&amp;A2&amp;" --no-hd --no-sq --no-unal")</f>
@@ -8976,10 +8626,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>979</v>
+        <v>910</v>
       </c>
       <c r="C3" t="s">
-        <v>980</v>
+        <v>911</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
@@ -8988,10 +8638,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>981</v>
+        <v>912</v>
       </c>
       <c r="C4" t="s">
-        <v>982</v>
+        <v>913</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -9000,10 +8650,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>983</v>
+        <v>914</v>
       </c>
       <c r="C5" t="s">
-        <v>984</v>
+        <v>915</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -9012,10 +8662,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>985</v>
+        <v>916</v>
       </c>
       <c r="C6" t="s">
-        <v>986</v>
+        <v>917</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -9024,10 +8674,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>987</v>
+        <v>918</v>
       </c>
       <c r="C7" t="s">
-        <v>988</v>
+        <v>919</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -9036,10 +8686,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>989</v>
+        <v>920</v>
       </c>
       <c r="C8" t="s">
-        <v>990</v>
+        <v>921</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -9048,10 +8698,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>991</v>
+        <v>922</v>
       </c>
       <c r="C9" t="s">
-        <v>992</v>
+        <v>923</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -9060,10 +8710,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>993</v>
+        <v>924</v>
       </c>
       <c r="C10" t="s">
-        <v>994</v>
+        <v>925</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -9072,10 +8722,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>995</v>
+        <v>926</v>
       </c>
       <c r="C11" t="s">
-        <v>996</v>
+        <v>927</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -9084,10 +8734,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>997</v>
+        <v>928</v>
       </c>
       <c r="C12" t="s">
-        <v>998</v>
+        <v>929</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -9096,10 +8746,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>999</v>
+        <v>930</v>
       </c>
       <c r="C13" t="s">
-        <v>1000</v>
+        <v>931</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -9108,10 +8758,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>1001</v>
+        <v>932</v>
       </c>
       <c r="C14" t="s">
-        <v>1002</v>
+        <v>933</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -9120,10 +8770,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1003</v>
+        <v>934</v>
       </c>
       <c r="C15" t="s">
-        <v>1004</v>
+        <v>935</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -9132,10 +8782,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1005</v>
+        <v>936</v>
       </c>
       <c r="C16" t="s">
-        <v>1006</v>
+        <v>937</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -9144,10 +8794,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1007</v>
+        <v>938</v>
       </c>
       <c r="C17" t="s">
-        <v>1008</v>
+        <v>939</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -9156,10 +8806,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>1009</v>
+        <v>940</v>
       </c>
       <c r="C18" t="s">
-        <v>1010</v>
+        <v>941</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -9168,10 +8818,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1011</v>
+        <v>942</v>
       </c>
       <c r="C19" t="s">
-        <v>1012</v>
+        <v>943</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -9180,10 +8830,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1013</v>
+        <v>944</v>
       </c>
       <c r="C20" t="s">
-        <v>1014</v>
+        <v>945</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -9192,10 +8842,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>1015</v>
+        <v>946</v>
       </c>
       <c r="C21" t="s">
-        <v>1016</v>
+        <v>947</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -9204,10 +8854,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>1017</v>
+        <v>948</v>
       </c>
       <c r="C22" t="s">
-        <v>1018</v>
+        <v>949</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -9216,10 +8866,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>1019</v>
+        <v>950</v>
       </c>
       <c r="C23" t="s">
-        <v>1020</v>
+        <v>951</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -9228,117 +8878,117 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>1021</v>
+        <v>952</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>1022</v>
+        <v>953</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>1023</v>
+        <v>954</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>1024</v>
+        <v>955</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>1025</v>
+        <v>956</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>1026</v>
+        <v>957</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>1027</v>
+        <v>958</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>1028</v>
+        <v>959</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>1029</v>
+        <v>960</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>1030</v>
+        <v>961</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>1031</v>
+        <v>962</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>1032</v>
+        <v>963</v>
       </c>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>1033</v>
+        <v>964</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>1034</v>
+        <v>965</v>
       </c>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>1035</v>
+        <v>966</v>
       </c>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>1036</v>
+        <v>967</v>
       </c>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>1037</v>
+        <v>968</v>
       </c>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>1038</v>
+        <v>969</v>
       </c>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>1039</v>
+        <v>970</v>
       </c>
     </row>
     <row r="43" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>1040</v>
+        <v>971</v>
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>1041</v>
+        <v>972</v>
       </c>
     </row>
     <row r="45" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>1042</v>
+        <v>973</v>
       </c>
     </row>
     <row r="46" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>1043</v>
+        <v>974</v>
       </c>
     </row>
   </sheetData>

</xml_diff>